<commit_message>
update kklhp , pilih , etc
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -10,12 +10,15 @@
     <sheet name="TLHP" sheetId="1" r:id="rId1"/>
     <sheet name="coding" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$46</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>TLHP</t>
   </si>
@@ -29,27 +32,48 @@
     <t>link</t>
   </si>
   <si>
+    <t>kklhp add row temuan</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kklhp add row rekomendasi </t>
+  </si>
+  <si>
+    <t>kklhp insert to db</t>
+  </si>
+  <si>
+    <t>Edit LHP Menu</t>
+  </si>
+  <si>
     <t>call reprosess after insert / update manus datatable</t>
   </si>
   <si>
-    <t>Add tim</t>
+    <t>Add tim coding</t>
   </si>
   <si>
     <t>datatable get manus</t>
   </si>
   <si>
-    <t>ci tlhp ... done</t>
-  </si>
-  <si>
-    <t>ci dashboard ... done</t>
-  </si>
-  <si>
-    <t>=-datepicker</t>
+    <t>ci tlhp</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ci dashboard </t>
+  </si>
+  <si>
+    <t>datepicker style hover and active</t>
   </si>
   <si>
     <t>modal for add user</t>
   </si>
   <si>
+    <t>agus</t>
+  </si>
+  <si>
     <t>modal for edit user</t>
   </si>
   <si>
@@ -59,7 +83,7 @@
     <t>Electronic follow up recommendation (index.php) &amp; RB</t>
   </si>
   <si>
-    <t>index dashboard tlhp legend on pie chart</t>
+    <t>index dashboard tlhp legend on pie chart for printing</t>
   </si>
   <si>
     <t>footer add logo kemenpan</t>
@@ -120,9 +144,6 @@
   </si>
   <si>
     <t xml:space="preserve">bug on datepicker klik field tanggal addlhp </t>
-  </si>
-  <si>
-    <t>done</t>
   </si>
   <si>
     <t>css upload addlhp</t>
@@ -162,7 +183,14 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,159 +648,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1089,11 +1117,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:E44"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1118,208 +1148,276 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:2">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="2" t="s">
-        <v>9</v>
+      <c r="B7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" hidden="1" spans="2:3">
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" hidden="1" spans="2:3">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" hidden="1" spans="2:4">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" hidden="1" spans="2:4">
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" hidden="1" spans="2:3">
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" hidden="1" spans="2:3">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" hidden="1" spans="2:3">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" hidden="1" spans="2:3">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="2:3">
+      <c r="D31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
       <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" hidden="1" spans="2:3">
       <c r="B35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" hidden="1" spans="2:3">
       <c r="B36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
         <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C46">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="equal" val=""/>
+        <customFilter operator="equal" val="progress"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E28" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
+    <hyperlink ref="E32" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1337,7 +1435,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lhp & kklhp update
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -11,14 +11,14 @@
     <sheet name="coding" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$49</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
   <si>
     <t>TLHP</t>
   </si>
@@ -32,6 +32,9 @@
     <t>link</t>
   </si>
   <si>
+    <t>Bug ON after add tr rekomen / add more get from last so inputan nya masi ke bawa</t>
+  </si>
+  <si>
     <t>kklhp add row temuan</t>
   </si>
   <si>
@@ -50,7 +53,10 @@
     <t>call reprosess after insert / update manus datatable</t>
   </si>
   <si>
-    <t>Add tim coding</t>
+    <t>Add tim coding post</t>
+  </si>
+  <si>
+    <t>add tim disable double</t>
   </si>
   <si>
     <t>datatable get manus</t>
@@ -125,10 +131,13 @@
     <t>CSS</t>
   </si>
   <si>
+    <t>hari penugasan perpanjangan kolum date nya tidak sama</t>
+  </si>
+  <si>
+    <t>alfon</t>
+  </si>
+  <si>
     <t>header make smaller</t>
-  </si>
-  <si>
-    <t>alfon</t>
   </si>
   <si>
     <t xml:space="preserve">dashboard app make like </t>
@@ -1118,12 +1127,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1148,33 +1157,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:2">
@@ -1192,68 +1201,65 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" hidden="1" spans="2:3">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" hidden="1" spans="2:3">
-      <c r="B10" t="s">
+    <row r="11" hidden="1" spans="2:3">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" hidden="1" spans="2:4">
+    <row r="12" hidden="1" spans="2:3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" hidden="1" spans="2:4">
-      <c r="B13" t="s">
+    <row r="14" hidden="1" spans="2:4">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" hidden="1" spans="2:3">
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" hidden="1" spans="2:3">
+    </row>
+    <row r="15" hidden="1" spans="2:4">
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" hidden="1" spans="2:3">
       <c r="B16" t="s">
         <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" hidden="1" spans="2:3">
@@ -1261,7 +1267,7 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:2">
@@ -1269,9 +1275,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" hidden="1" spans="2:3">
       <c r="B19" t="s">
         <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:2">
@@ -1284,12 +1293,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" hidden="1" spans="2:3">
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
         <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:2">
@@ -1297,9 +1303,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" hidden="1" spans="2:3">
       <c r="B24" t="s">
         <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:2">
@@ -1322,90 +1331,129 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
-      <c r="B31" t="s">
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
         <v>35</v>
       </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="B32" t="s">
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" hidden="1" spans="2:3">
-      <c r="B35" t="s">
+      <c r="D35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" hidden="1" spans="2:3">
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
+      <c r="D36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
       <c r="B37" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="2:2">
+      <c r="D37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" hidden="1" spans="2:3">
       <c r="B38" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="2:2">
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" hidden="1" spans="2:3">
       <c r="B39" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="2:2">
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
       <c r="B40" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
+      <c r="D40" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
+      <c r="D41" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
+      <c r="D42" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" t="s">
         <v>49</v>
       </c>
+      <c r="D43" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C46">
+  <autoFilter ref="C1:C49">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="equal" val=""/>
@@ -1414,7 +1462,7 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E32" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
+    <hyperlink ref="E35" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1435,7 +1483,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
repair dashboard & url
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -11,14 +11,14 @@
     <sheet name="coding" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$51</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
   <si>
     <t>TLHP</t>
   </si>
@@ -35,6 +35,12 @@
     <t>Insert Kode Sebab, Uraian, Temuan</t>
   </si>
   <si>
+    <t xml:space="preserve">User Authentication </t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>Bug ON after add tr rekomen / add more get from last so inputan nya masi ke bawa</t>
   </si>
   <si>
@@ -66,9 +72,6 @@
   </si>
   <si>
     <t>ci tlhp</t>
-  </si>
-  <si>
-    <t>done</t>
   </si>
   <si>
     <t xml:space="preserve">ci dashboard </t>
@@ -811,11 +814,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
@@ -1139,12 +1145,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1174,16 +1180,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
+    <row r="3" hidden="1" spans="2:3">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:3">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1191,48 +1197,48 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
+    </row>
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" hidden="1" spans="2:3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1241,68 +1247,71 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" hidden="1" spans="2:3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" hidden="1" spans="2:4">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="16" hidden="1" spans="2:4">
       <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" hidden="1" spans="2:3">
+    </row>
+    <row r="17" hidden="1" spans="2:4">
       <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" hidden="1" spans="2:3">
       <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" hidden="1" spans="2:3">
       <c r="B19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" hidden="1" spans="2:3">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
+    </row>
+    <row r="21" hidden="1" spans="2:3">
       <c r="B21" t="s">
         <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:2">
@@ -1320,17 +1329,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" hidden="1" spans="2:3">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
+    </row>
+    <row r="26" hidden="1" spans="2:3">
       <c r="B26" t="s">
         <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:2">
@@ -1358,60 +1367,57 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
-      <c r="B34" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>38</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" t="s">
+      <c r="D37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" hidden="1" spans="2:3">
+      <c r="D38" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>45</v>
       </c>
-      <c r="C39" t="s">
-        <v>16</v>
+      <c r="D39" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="40" hidden="1" spans="2:3">
@@ -1419,44 +1425,47 @@
         <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" hidden="1" spans="2:3">
       <c r="B41" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>39</v>
+      <c r="C41" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>39</v>
+      <c r="D42" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>39</v>
+      <c r="D43" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
+      <c r="D44" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" t="s">
         <v>51</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -1469,8 +1478,13 @@
         <v>53</v>
       </c>
     </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C50">
+  <autoFilter ref="C1:C51">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="equal" val=""/>
@@ -1479,7 +1493,7 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E36" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
+    <hyperlink ref="E37" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1500,7 +1514,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change textarea user address
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -11,14 +11,14 @@
     <sheet name="coding" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$55</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
   <si>
     <t>TLHP</t>
   </si>
@@ -29,30 +29,36 @@
     <t>assignment</t>
   </si>
   <si>
+    <t>desc</t>
+  </si>
+  <si>
     <t>link</t>
   </si>
   <si>
     <t>Repair User password add edit add repassword</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>require re pass if pass input in edit</t>
+  </si>
+  <si>
     <t>Insert Kode Sebab, Uraian, Temuan</t>
   </si>
   <si>
+    <t>progress</t>
+  </si>
+  <si>
     <t xml:space="preserve">User Authentication </t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Bug ON after add tr rekomen / add more get from last so inputan nya masi ke bawa</t>
   </si>
   <si>
     <t>kklhp add row temuan</t>
   </si>
   <si>
-    <t>progress</t>
-  </si>
-  <si>
     <t xml:space="preserve">kklhp add row rekomendasi </t>
   </si>
   <si>
@@ -168,6 +174,9 @@
   </si>
   <si>
     <t>css upload addlhp</t>
+  </si>
+  <si>
+    <t>panah atas bawah di datatable</t>
   </si>
   <si>
     <t>bootstrap loading gif when load url</t>
@@ -1157,23 +1166,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="5.75" customWidth="1"/>
     <col min="2" max="2" width="102.375" customWidth="1"/>
     <col min="4" max="4" width="10.875" customWidth="1"/>
-    <col min="5" max="5" width="79.125" customWidth="1"/>
+    <col min="5" max="5" width="31.25" customWidth="1"/>
+    <col min="6" max="6" width="79.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,335 +1196,368 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="2:2">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" hidden="1" spans="2:3">
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" hidden="1" spans="2:3">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" hidden="1" spans="2:3">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" hidden="1" spans="2:4">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" hidden="1" spans="2:4">
       <c r="B18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" hidden="1" spans="2:3">
       <c r="B19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" hidden="1" spans="2:3">
       <c r="B20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" hidden="1" spans="2:3">
       <c r="B22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" hidden="1" spans="2:3">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
       <c r="B37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E37" s="3"/>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
       <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
+      <c r="E39" s="3"/>
+      <c r="F39" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
       <c r="B40" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
+        <v>44</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="2:5">
       <c r="B41" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E41" s="3"/>
     </row>
     <row r="42" hidden="1" spans="2:3">
       <c r="B42" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" hidden="1" spans="2:3">
       <c r="B43" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4">
+        <v>52</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="2:6">
       <c r="B45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4">
+        <v>44</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
       <c r="B46" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4">
+        <v>44</v>
+      </c>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="2:5">
       <c r="B47" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4">
+        <v>44</v>
+      </c>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="2:5">
       <c r="B48" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="3"/>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C54">
+  <autoFilter ref="C1:C55">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="equal" val=""/>
@@ -1523,7 +1566,7 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E39" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
+    <hyperlink ref="F39" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1544,7 +1587,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error 404 routes home
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13350"/>
+    <workbookView windowWidth="28695" windowHeight="13350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TLHP" sheetId="1" r:id="rId1"/>
     <sheet name="coding" sheetId="2" r:id="rId2"/>
+    <sheet name="clear" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$C$1:$C$62</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72">
   <si>
     <t>TLHP</t>
   </si>
@@ -225,6 +226,15 @@
   </si>
   <si>
     <t>create php check if date and auto re format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database blaba </t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copyright </t>
   </si>
 </sst>
 </file>
@@ -597,12 +607,117 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -738,7 +853,7 @@
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -780,10 +895,10 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -792,22 +907,22 @@
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -819,7 +934,7 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -840,22 +955,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -1186,10 +1331,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1230,7 +1375,7 @@
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -1238,7 +1383,7 @@
       </c>
     </row>
     <row r="4" hidden="1" spans="2:3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
@@ -1264,7 +1409,7 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1272,7 +1417,7 @@
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1356,7 +1501,7 @@
       <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1473,10 +1618,10 @@
       <c r="B44" t="s">
         <v>49</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" t="s">
@@ -1490,11 +1635,11 @@
       <c r="B46" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="4" t="s">
+      <c r="E46" s="13"/>
+      <c r="F46" s="14" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1502,19 +1647,19 @@
       <c r="B47" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="3"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="3"/>
+      <c r="E48" s="13"/>
     </row>
     <row r="49" hidden="1" spans="2:3">
       <c r="B49" t="s">
@@ -1536,19 +1681,19 @@
       <c r="B51" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E51" s="3"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E52" s="3"/>
+      <c r="E52" s="13"/>
       <c r="F52" t="s">
         <v>60</v>
       </c>
@@ -1557,37 +1702,37 @@
       <c r="B53" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E53" s="3"/>
+      <c r="E53" s="13"/>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="E54" s="13"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="13"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E56" s="3"/>
+      <c r="E56" s="13"/>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
@@ -1642,4 +1787,54 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="C3:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="14.25"/>
+    <row r="4" spans="3:3">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="8" spans="9:11">
+      <c r="I8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="9:11">
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" ht="14.25" spans="9:11">
+      <c r="I10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="I8:J9"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add current app detect
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -12,14 +12,14 @@
     <sheet name="clear" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$D$1:$D$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$D$1:$D$73</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
   <si>
     <t>TLHP</t>
   </si>
@@ -51,6 +51,21 @@
     <t>input normal form kklhp</t>
   </si>
   <si>
+    <t>header current App</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>haidar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header fullname </t>
+  </si>
+  <si>
+    <t>Header, footer, logo current app</t>
+  </si>
+  <si>
     <t>Input tindak lanjut</t>
   </si>
   <si>
@@ -63,25 +78,28 @@
     <t>progress</t>
   </si>
   <si>
+    <t>using error/ folder and change header &amp; footer</t>
+  </si>
+  <si>
     <t>Repair User password add edit add repassword</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>require re pass if pass input in edit</t>
   </si>
   <si>
     <t>Insert Kode Sebab, Uraian, Temuan using csv</t>
   </si>
   <si>
+    <t>medium</t>
+  </si>
+  <si>
     <t xml:space="preserve">User Authentication </t>
   </si>
   <si>
     <t>Bug ON after add tr rekomen / add more get from last so inputan nya masi ke bawa</t>
   </si>
   <si>
-    <t>medium</t>
+    <t>total use login logout</t>
   </si>
   <si>
     <t>Cetak Print</t>
@@ -94,9 +112,6 @@
   </si>
   <si>
     <t>Create Tables for 4 app</t>
-  </si>
-  <si>
-    <t>haidar</t>
   </si>
   <si>
     <t>Create Multi App login &amp; tables</t>
@@ -449,12 +464,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -865,130 +886,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1003,14 +1024,14 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1044,13 +1065,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43" applyFont="1">
@@ -1371,12 +1398,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1385,7 +1412,7 @@
     <col min="2" max="2" width="102.375" customWidth="1"/>
     <col min="3" max="3" width="6.875" customWidth="1"/>
     <col min="5" max="5" width="10.875" customWidth="1"/>
-    <col min="6" max="6" width="31.25" customWidth="1"/>
+    <col min="6" max="6" width="41.875" customWidth="1"/>
     <col min="7" max="7" width="79.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1410,10 +1437,10 @@
       </c>
     </row>
     <row r="2" spans="2:3">
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1421,7 +1448,7 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1429,580 +1456,624 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" hidden="1" spans="2:5">
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="E6" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" hidden="1" spans="2:6">
+    </row>
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C8" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" hidden="1" spans="2:4">
-      <c r="B10" s="13" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" hidden="1" spans="2:6">
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" t="s">
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>20</v>
+      <c r="C12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" hidden="1" spans="2:4">
+      <c r="B13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
+    </row>
+    <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
+        <v>26</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="2:5">
+      <c r="C16" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="C17" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
+      <c r="C18" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" hidden="1" spans="2:5">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
+      <c r="C19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" hidden="1" spans="2:5">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" t="s">
+      <c r="D20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
+      <c r="D22" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" hidden="1" spans="2:4">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" hidden="1" spans="2:4">
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="D25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" hidden="1" spans="2:4">
+      <c r="C25" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" hidden="1" spans="2:5">
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" hidden="1" spans="2:5">
+    </row>
+    <row r="28" hidden="1" spans="2:4">
       <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" hidden="1" spans="2:5">
+        <v>42</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" hidden="1" spans="2:4">
       <c r="B29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" hidden="1" spans="2:5">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" hidden="1" spans="2:4">
       <c r="B30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" hidden="1" spans="2:5">
       <c r="B31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="32" hidden="1" spans="2:5">
       <c r="B32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" hidden="1" spans="2:5">
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>20</v>
+      <c r="D33" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" hidden="1" spans="2:5">
       <c r="B34" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>46</v>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
         <v>49</v>
       </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
+      <c r="C35" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" hidden="1" spans="2:5">
       <c r="B36" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" hidden="1" spans="2:4">
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
       <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" hidden="1" spans="2:5">
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
+    </row>
+    <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" hidden="1" spans="2:4">
       <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>29</v>
+        <v>56</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>29</v>
+      <c r="E42" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
+      <c r="E43" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
       <c r="B46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
+        <v>61</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
       <c r="B47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" hidden="1" spans="2:5">
+      <c r="E47" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" hidden="1" spans="2:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F51" s="11"/>
-    </row>
-    <row r="52" hidden="1" spans="2:5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>64</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
       <c r="B53" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="54" hidden="1" spans="2:6">
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" hidden="1" spans="2:5">
       <c r="B54" t="s">
         <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F54" s="11"/>
-    </row>
-    <row r="55" spans="2:6">
+        <v>11</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" hidden="1" spans="2:6">
       <c r="B55" t="s">
         <v>68</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F55" s="11"/>
-    </row>
-    <row r="56" hidden="1" spans="2:4">
+      <c r="D55" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" hidden="1" spans="2:5">
       <c r="B56" t="s">
         <v>69</v>
       </c>
-      <c r="D56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" hidden="1" spans="2:4">
+      <c r="D56" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
       <c r="B57" t="s">
         <v>70</v>
       </c>
-      <c r="D57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6">
+      <c r="E57" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" hidden="1" spans="2:6">
       <c r="B58" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" s="11"/>
-    </row>
-    <row r="59" spans="2:7">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F58" s="12"/>
+    </row>
+    <row r="59" spans="2:6">
       <c r="B59" t="s">
-        <v>72</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" s="11"/>
-      <c r="G59" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="2:6">
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" hidden="1" spans="2:4">
       <c r="B60" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F60" s="11"/>
-    </row>
-    <row r="61" hidden="1" spans="2:6">
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" hidden="1" spans="2:4">
       <c r="B61" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F61" s="11"/>
-    </row>
-    <row r="62" hidden="1" spans="2:6">
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
       <c r="B62" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E62" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" s="11"/>
-    </row>
-    <row r="63" hidden="1" spans="2:6">
+      <c r="E62" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="2:7">
       <c r="B63" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F63" s="11"/>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
+      <c r="E63" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" s="12"/>
+      <c r="G63" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
+    <row r="64" spans="2:6">
+      <c r="B64" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+      <c r="E64" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" hidden="1" spans="2:6">
+      <c r="B65" t="s">
         <v>80</v>
       </c>
+      <c r="D65" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" hidden="1" spans="2:6">
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" hidden="1" spans="2:6">
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D69">
+  <autoFilter ref="D1:D73">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="equal" val=""/>
@@ -2011,7 +2082,7 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="G53" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
+    <hyperlink ref="G57" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2032,7 +2103,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2061,11 +2132,11 @@
     </row>
     <row r="8" spans="9:11">
       <c r="I8" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="9:11">
@@ -2075,14 +2146,14 @@
     </row>
     <row r="10" ht="14.25" spans="9:11">
       <c r="I10" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
     <row r="27" spans="8:8">
       <c r="H27" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new task & ignore something
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -1401,9 +1401,9 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1436,7 +1436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
+    <row r="2" hidden="1" spans="2:3">
       <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" hidden="1" spans="2:3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" hidden="1" spans="2:3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" hidden="1" spans="2:5">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" hidden="1" spans="2:3">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" hidden="1" spans="2:3">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" hidden="1" spans="2:3">
       <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" hidden="1" spans="2:3">
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" hidden="1" spans="2:3">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" hidden="1" spans="2:3">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" hidden="1" spans="2:3">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" hidden="1" spans="2:3">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1619,40 +1619,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" hidden="1" spans="2:5">
       <c r="B21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" hidden="1" spans="2:5">
       <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" hidden="1" spans="2:5">
       <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
       <c r="E23" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" hidden="1" spans="2:5">
       <c r="B24" t="s">
         <v>37</v>
       </c>
@@ -1663,7 +1656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" hidden="1" spans="2:3">
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -1671,7 +1664,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" hidden="1" spans="2:3">
       <c r="B26" t="s">
         <v>40</v>
       </c>
@@ -1679,7 +1672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" hidden="1" spans="2:3">
       <c r="B27" t="s">
         <v>41</v>
       </c>
@@ -1755,7 +1748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" hidden="1" spans="2:3">
       <c r="B35" t="s">
         <v>49</v>
       </c>
@@ -1774,7 +1767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" hidden="1" spans="2:3">
       <c r="B37" t="s">
         <v>52</v>
       </c>
@@ -1793,7 +1786,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" hidden="1" spans="2:3">
       <c r="B39" t="s">
         <v>54</v>
       </c>
@@ -1801,7 +1794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" hidden="1" spans="2:2">
       <c r="B40" t="s">
         <v>55</v>
       </c>
@@ -1814,7 +1807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" hidden="1" spans="2:5">
       <c r="B42" t="s">
         <v>57</v>
       </c>
@@ -1825,7 +1818,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" hidden="1" spans="2:5">
       <c r="B43" t="s">
         <v>58</v>
       </c>
@@ -1836,7 +1829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" hidden="1" spans="2:5">
       <c r="B44" t="s">
         <v>59</v>
       </c>
@@ -1847,7 +1840,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" hidden="1" spans="2:5">
       <c r="B45" t="s">
         <v>60</v>
       </c>
@@ -1858,7 +1851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" hidden="1" spans="2:5">
       <c r="B46" t="s">
         <v>61</v>
       </c>
@@ -1869,7 +1862,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" hidden="1" spans="2:5">
       <c r="B47" t="s">
         <v>62</v>
       </c>
@@ -1880,22 +1873,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
+    <row r="48" hidden="1"/>
+    <row r="49" hidden="1"/>
+    <row r="50" hidden="1" spans="2:2">
       <c r="B50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" hidden="1" spans="2:2">
       <c r="B51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" hidden="1" spans="2:2">
       <c r="B52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" hidden="1" spans="2:5">
       <c r="B53" t="s">
         <v>66</v>
       </c>
@@ -1941,7 +1936,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" hidden="1" spans="2:7">
       <c r="B57" t="s">
         <v>70</v>
       </c>
@@ -1965,7 +1960,7 @@
       </c>
       <c r="F58" s="12"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" hidden="1" spans="2:6">
       <c r="B59" t="s">
         <v>73</v>
       </c>
@@ -1991,7 +1986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" hidden="1" spans="2:6">
       <c r="B62" t="s">
         <v>76</v>
       </c>
@@ -2000,7 +1995,7 @@
       </c>
       <c r="F62" s="12"/>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" hidden="1" spans="2:7">
       <c r="B63" t="s">
         <v>77</v>
       </c>
@@ -2012,7 +2007,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" hidden="1" spans="2:6">
       <c r="B64" t="s">
         <v>79</v>
       </c>
@@ -2057,17 +2052,20 @@
       </c>
       <c r="F67" s="12"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="68" hidden="1"/>
+    <row r="69" hidden="1"/>
+    <row r="70" hidden="1"/>
+    <row r="71" hidden="1" spans="1:1">
       <c r="A71" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" hidden="1" spans="1:1">
       <c r="A72" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" hidden="1" spans="1:1">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -2076,7 +2074,6 @@
   <autoFilter ref="D1:D73">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter operator="equal" val=""/>
         <customFilter operator="equal" val="progress"/>
       </customFilters>
     </filterColumn>

</xml_diff>

<commit_message>
repair merge dendi kklhp coding
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
   <si>
     <t>TLHP</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>medium</t>
+  </si>
+  <si>
+    <t>rudi</t>
   </si>
   <si>
     <t xml:space="preserve">User Authentication </t>
@@ -1424,7 +1427,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1610,7 +1613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:5">
       <c r="B18" s="15" t="s">
         <v>31</v>
       </c>
@@ -1620,10 +1623,13 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" hidden="1" spans="2:4">
       <c r="B19" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" t="s">
@@ -1632,7 +1638,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>32</v>
@@ -1640,7 +1646,7 @@
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
@@ -1648,7 +1654,7 @@
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1656,7 +1662,7 @@
     </row>
     <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -1664,7 +1670,7 @@
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -1672,7 +1678,7 @@
     </row>
     <row r="25" hidden="1" spans="2:5">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -1686,47 +1692,47 @@
     </row>
     <row r="26" hidden="1" spans="2:5">
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
         <v>45</v>
-      </c>
-      <c r="E29" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="2:3">
       <c r="B31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -1734,7 +1740,7 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
@@ -1745,7 +1751,7 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -1753,7 +1759,7 @@
     </row>
     <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
         <v>32</v>
@@ -1761,7 +1767,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
@@ -1769,7 +1775,7 @@
     </row>
     <row r="36" hidden="1" spans="2:4">
       <c r="B36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
@@ -1777,7 +1783,7 @@
     </row>
     <row r="37" hidden="1" spans="2:4">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -1785,7 +1791,7 @@
     </row>
     <row r="38" hidden="1" spans="2:4">
       <c r="B38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
@@ -1793,29 +1799,29 @@
     </row>
     <row r="39" hidden="1" spans="2:5">
       <c r="B39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" hidden="1" spans="2:5">
       <c r="B40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" hidden="1" spans="2:5">
       <c r="B41" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -1826,7 +1832,7 @@
     </row>
     <row r="42" hidden="1" spans="2:5">
       <c r="B42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -1837,7 +1843,7 @@
     </row>
     <row r="43" spans="2:3">
       <c r="B43" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
         <v>32</v>
@@ -1845,18 +1851,18 @@
     </row>
     <row r="44" hidden="1" spans="2:5">
       <c r="B44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
         <v>32</v>
@@ -1864,18 +1870,18 @@
     </row>
     <row r="46" hidden="1" spans="2:5">
       <c r="B46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>32</v>
@@ -1883,12 +1889,12 @@
     </row>
     <row r="48" spans="2:2">
       <c r="B48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" hidden="1" spans="2:4">
       <c r="B49" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
@@ -1896,163 +1902,163 @@
     </row>
     <row r="50" spans="2:5">
       <c r="B50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="2:2">
       <c r="B58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" hidden="1" spans="2:5">
       <c r="B61" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" hidden="1" spans="2:5">
       <c r="B62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" hidden="1" spans="2:5">
       <c r="B63" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="2:8">
       <c r="B64" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" hidden="1" spans="2:5">
       <c r="B65" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="2:5">
       <c r="B66" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E66" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" hidden="1" spans="2:4">
       <c r="B67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D67" t="s">
         <v>17</v>
@@ -2060,7 +2066,7 @@
     </row>
     <row r="68" hidden="1" spans="2:4">
       <c r="B68" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
@@ -2068,77 +2074,77 @@
     </row>
     <row r="69" spans="2:5">
       <c r="B69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E69" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="2:8">
       <c r="B70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E70" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H70" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="2:5">
       <c r="B71" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E71" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" hidden="1" spans="2:5">
       <c r="B72" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" hidden="1" spans="2:5">
       <c r="B73" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" hidden="1" spans="2:5">
       <c r="B74" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D74" t="s">
         <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2172,7 +2178,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2201,11 +2207,11 @@
     <row r="7" ht="14.25"/>
     <row r="8" spans="9:11">
       <c r="I8" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" ht="14.25" spans="9:11">
@@ -2215,14 +2221,14 @@
     </row>
     <row r="10" ht="14.25" spans="9:11">
       <c r="I10" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
     <row r="27" spans="8:8">
       <c r="H27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kklhp bug for update good on first insert
</commit_message>
<xml_diff>
--- a/e4/assets/task.xlsx
+++ b/e4/assets/task.xlsx
@@ -12,14 +12,14 @@
     <sheet name="clear" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$D$1:$D$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TLHP!$D$1:$D$82</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103">
   <si>
     <t>TLHP</t>
   </si>
@@ -51,6 +51,9 @@
     <t>bug on user history</t>
   </si>
   <si>
+    <t>KKLHP bug if edit cannot add button more in a b c</t>
+  </si>
+  <si>
     <t>Summernote upload to file system</t>
   </si>
   <si>
@@ -60,21 +63,30 @@
     <t>Summernote</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>rudi</t>
+  </si>
+  <si>
+    <t>Page Template Laporan</t>
+  </si>
+  <si>
     <t>progress</t>
   </si>
   <si>
-    <t>Page Template Laporan</t>
-  </si>
-  <si>
     <t>Log History</t>
   </si>
   <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>agus</t>
+  </si>
+  <si>
     <t>Console error</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>hari awal tidak boleh lebih dari hari akhir</t>
   </si>
   <si>
@@ -120,12 +132,6 @@
     <t>Insert Kode Sebab, Uraian, Temuan using csv</t>
   </si>
   <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>rudi</t>
-  </si>
-  <si>
     <t xml:space="preserve">User Authentication </t>
   </si>
   <si>
@@ -148,9 +154,6 @@
   </si>
   <si>
     <t>Create Multi App login &amp; tables</t>
-  </si>
-  <si>
-    <t>agus</t>
   </si>
   <si>
     <t>upload jquery</t>
@@ -1425,12 +1428,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1483,252 +1486,262 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="12" t="s">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" hidden="1" spans="2:4">
-      <c r="B8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="11" t="s">
+    <row r="8" spans="2:5">
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" hidden="1" spans="2:4">
+      <c r="B9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11"/>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
+      <c r="B10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" hidden="1" spans="2:5">
+    <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5">
+    </row>
+    <row r="13" hidden="1" spans="2:5">
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
       <c r="E13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>8</v>
       </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="15" t="s">
-        <v>26</v>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" hidden="1" spans="2:7">
+    <row r="17" spans="2:3">
       <c r="B17" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" hidden="1" spans="2:6">
-      <c r="B18" t="s">
-        <v>30</v>
+    </row>
+    <row r="18" hidden="1" spans="2:7">
+      <c r="B18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G18" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="19" hidden="1" spans="2:6">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
       <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" hidden="1" spans="2:4">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
       <c r="D20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" hidden="1" spans="2:4">
+      <c r="B21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" hidden="1" spans="2:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" hidden="1" spans="2:5">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" hidden="1" spans="2:5">
       <c r="B28" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="2:5">
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
         <v>45</v>
       </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
         <v>47</v>
-      </c>
-      <c r="E30" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:5">
@@ -1736,34 +1749,34 @@
         <v>48</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
       <c r="B32" t="s">
         <v>49</v>
       </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
       <c r="B34" t="s">
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="2:3">
@@ -1771,7 +1784,7 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:3">
@@ -1779,15 +1792,15 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" hidden="1" spans="2:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
       <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="D37" t="s">
-        <v>17</v>
+      <c r="C37" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" hidden="1" spans="2:4">
@@ -1795,7 +1808,7 @@
         <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" hidden="1" spans="2:4">
@@ -1803,18 +1816,15 @@
         <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" hidden="1" spans="2:5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" hidden="1" spans="2:4">
       <c r="B40" t="s">
         <v>57</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" hidden="1" spans="2:5">
@@ -1822,10 +1832,10 @@
         <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" hidden="1" spans="2:5">
@@ -1833,10 +1843,10 @@
         <v>59</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" hidden="1" spans="2:5">
@@ -1844,80 +1854,80 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" hidden="1" spans="2:5">
       <c r="B44" t="s">
         <v>61</v>
       </c>
-      <c r="C44" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" hidden="1" spans="2:5">
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
       <c r="B45" t="s">
         <v>62</v>
       </c>
-      <c r="D45" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" hidden="1" spans="2:5">
+      <c r="B46" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" t="s">
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
         <v>64</v>
       </c>
-      <c r="C46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" hidden="1" spans="2:5">
+    </row>
+    <row r="47" spans="2:3">
       <c r="B47" t="s">
         <v>65</v>
       </c>
-      <c r="D47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" hidden="1" spans="2:5">
       <c r="B48" t="s">
         <v>66</v>
       </c>
-      <c r="C48" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
       <c r="B49" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" hidden="1" spans="2:4">
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
       <c r="B50" t="s">
         <v>68</v>
       </c>
-      <c r="D50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
+    </row>
+    <row r="51" hidden="1" spans="2:4">
       <c r="B51" t="s">
         <v>69</v>
       </c>
-      <c r="C51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" t="s">
-        <v>46</v>
+      <c r="D51" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="2:5">
@@ -1928,7 +1938,7 @@
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="2:5">
@@ -1939,7 +1949,7 @@
         <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="2:5">
@@ -1950,7 +1960,7 @@
         <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="2:5">
@@ -1961,7 +1971,7 @@
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="2:5">
@@ -1972,45 +1982,45 @@
         <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="60" spans="2:5">
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
       <c r="B60" t="s">
         <v>76</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" t="s">
         <v>77</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" hidden="1" spans="2:5">
+      <c r="E61" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5">
       <c r="B62" t="s">
         <v>78</v>
       </c>
-      <c r="D62" t="s">
-        <v>17</v>
+      <c r="C62" t="s">
+        <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" hidden="1" spans="2:5">
@@ -2018,10 +2028,10 @@
         <v>79</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" hidden="1" spans="2:5">
@@ -2029,48 +2039,51 @@
         <v>80</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" hidden="1" spans="2:5">
       <c r="B65" t="s">
         <v>81</v>
       </c>
+      <c r="D65" t="s">
+        <v>14</v>
+      </c>
       <c r="E65" t="s">
-        <v>63</v>
-      </c>
-      <c r="H65" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="66" hidden="1" spans="2:5">
-      <c r="B66" t="s">
+      <c r="E66" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D66" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5">
+    </row>
+    <row r="67" hidden="1" spans="2:5">
       <c r="B67" t="s">
         <v>84</v>
       </c>
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
       <c r="E67" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" hidden="1" spans="2:4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
       <c r="B68" t="s">
         <v>85</v>
       </c>
-      <c r="D68" t="s">
-        <v>17</v>
+      <c r="E68" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="69" hidden="1" spans="2:4">
@@ -2078,45 +2091,42 @@
         <v>86</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" hidden="1" spans="2:4">
       <c r="B70" t="s">
         <v>87</v>
       </c>
-      <c r="E70" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8">
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
       <c r="B71" t="s">
         <v>88</v>
       </c>
       <c r="E71" t="s">
-        <v>63</v>
-      </c>
-      <c r="H71" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="72" spans="2:5">
-      <c r="B72" t="s">
+      <c r="E72" t="s">
+        <v>64</v>
+      </c>
+      <c r="H72" t="s">
         <v>90</v>
       </c>
-      <c r="E72" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" hidden="1" spans="2:5">
+    </row>
+    <row r="73" spans="2:5">
       <c r="B73" t="s">
         <v>91</v>
       </c>
-      <c r="D73" t="s">
-        <v>17</v>
-      </c>
       <c r="E73" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" hidden="1" spans="2:5">
@@ -2124,10 +2134,10 @@
         <v>92</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E74" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" hidden="1" spans="2:5">
@@ -2135,15 +2145,21 @@
         <v>93</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E75" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" hidden="1" spans="2:5">
+      <c r="B76" t="s">
         <v>94</v>
+      </c>
+      <c r="D76" t="s">
+        <v>14</v>
+      </c>
+      <c r="E76" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:1">
@@ -2156,8 +2172,13 @@
         <v>96</v>
       </c>
     </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="D1:D81">
+  <autoFilter ref="D1:D82">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="equal" val=""/>
@@ -2166,7 +2187,7 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="H65" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
+    <hyperlink ref="H66" r:id="rId1" display="http://demos.creative-tim.com/paper-dashboard-pro/examples/dashboard/overview.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2187,7 +2208,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2216,11 +2237,11 @@
     <row r="7" ht="14.25"/>
     <row r="8" spans="9:11">
       <c r="I8" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" ht="14.25" spans="9:11">
@@ -2230,14 +2251,14 @@
     </row>
     <row r="10" ht="14.25" spans="9:11">
       <c r="I10" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="10"/>
     </row>
     <row r="27" spans="8:8">
       <c r="H27" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>